<commit_message>
Conference Paper Commit 1
</commit_message>
<xml_diff>
--- a/validations/V8_Case_3.xlsx
+++ b/validations/V8_Case_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Classes\Research\Hephaestus\V_0.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Classes\Research\Hephaestus\V_021\AeroComBAT-Project\AeroComBAT-Project\validations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2587,11 +2587,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="474599328"/>
-        <c:axId val="474599720"/>
+        <c:axId val="210955352"/>
+        <c:axId val="210957312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474599328"/>
+        <c:axId val="210955352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,7 +2695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474599720"/>
+        <c:crossAx val="210957312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2703,7 +2703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474599720"/>
+        <c:axId val="210957312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2815,7 +2815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474599328"/>
+        <c:crossAx val="210955352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3739,8 +3739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,8 +4036,8 @@
         <v>0.47144258651410254</v>
       </c>
       <c r="AN3">
-        <f>(AF3-I3)/AF3*100</f>
-        <v>140.1057042264728</v>
+        <f>(AF3-H3)/AF3*100</f>
+        <v>-1.0681478297004339E-2</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
@@ -4145,8 +4145,8 @@
         <v>0.29708343302153567</v>
       </c>
       <c r="AN4">
-        <f t="shared" ref="AN4:AN42" si="11">(AF4-I4)/AF4*100</f>
-        <v>140.10581403380721</v>
+        <f t="shared" ref="AN4:AN42" si="11">(AF4-H4)/AF4*100</f>
+        <v>-1.0955302346561887E-2</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="AN5">
         <f t="shared" si="11"/>
-        <v>140.10592759228507</v>
+        <v>-1.1238480537006509E-2</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="AN6">
         <f t="shared" si="11"/>
-        <v>140.10604504323342</v>
+        <v>-1.1531365293345157E-2</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="AN7">
         <f t="shared" si="11"/>
-        <v>140.10616653217701</v>
+        <v>-1.1834319505675617E-2</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -4582,7 +4582,7 @@
       </c>
       <c r="AN8">
         <f t="shared" si="11"/>
-        <v>140.10629220870743</v>
+        <v>-1.2147716208404555E-2</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -4691,7 +4691,7 @@
       </c>
       <c r="AN9">
         <f t="shared" si="11"/>
-        <v>140.10642222629963</v>
+        <v>-1.2471938118159472E-2</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="AN10">
         <f t="shared" si="11"/>
-        <v>140.10655674206828</v>
+        <v>-1.2807377027999835E-2</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
@@ -4909,7 +4909,7 @@
       </c>
       <c r="AN11">
         <f t="shared" si="11"/>
-        <v>140.10669591645291</v>
+        <v>-1.315443302253173E-2</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -5018,7 +5018,7 @@
       </c>
       <c r="AN12">
         <f t="shared" si="11"/>
-        <v>140.10683991282266</v>
+        <v>-1.3513513491832446E-2</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -5127,7 +5127,7 @@
       </c>
       <c r="AN13">
         <f t="shared" si="11"/>
-        <v>140.1069888969885</v>
+        <v>-1.3885031913554651E-2</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="AN14">
         <f t="shared" si="11"/>
-        <v>140.10714303660666</v>
+        <v>-1.4269406370593277E-2</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="AN15">
         <f t="shared" si="11"/>
-        <v>140.10730250046601</v>
+        <v>-1.466705776562691E-2</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
@@ -5454,7 +5454,7 @@
       </c>
       <c r="AN16">
         <f t="shared" si="11"/>
-        <v>140.10746745763291</v>
+        <v>-1.5078407697312465E-2</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="AN17">
         <f t="shared" si="11"/>
-        <v>140.10763807644557</v>
+        <v>-1.5503875945811542E-2</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="AN18">
         <f t="shared" si="11"/>
-        <v>140.1078145233314</v>
+        <v>-1.594387752741952E-2</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="AN19">
         <f t="shared" si="11"/>
-        <v>140.10799696143022</v>
+        <v>-1.6398819260883841E-2</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
@@ -5890,7 +5890,7 @@
       </c>
       <c r="AN20">
         <f t="shared" si="11"/>
-        <v>140.10818554900089</v>
+        <v>-1.6869095791738568E-2</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="AN21">
         <f t="shared" si="11"/>
-        <v>140.10838043758417</v>
+        <v>-1.7355085014735053E-2</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="AN22">
         <f t="shared" si="11"/>
-        <v>140.10858176990203</v>
+        <v>-1.7857142831393481E-2</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
@@ -6217,7 +6217,7 @@
       </c>
       <c r="AN23">
         <f t="shared" si="11"/>
-        <v>140.10878967746248</v>
+        <v>-1.83755971807247E-2</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="AN24">
         <f t="shared" si="11"/>
-        <v>140.10900427784733</v>
+        <v>-1.8910741274330418E-2</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -6435,7 +6435,7 @@
       </c>
       <c r="AN25">
         <f t="shared" si="11"/>
-        <v>140.10922567165659</v>
+        <v>-1.9462825974922968E-2</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
@@ -6544,7 +6544,7 @@
       </c>
       <c r="AN26">
         <f t="shared" si="11"/>
-        <v>140.10945393908125</v>
+        <v>-2.0032051253844253E-2</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
@@ -6653,7 +6653,7 @@
       </c>
       <c r="AN27">
         <f t="shared" si="11"/>
-        <v>140.10968913608724</v>
+        <v>-2.0618556672122961E-2</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="AN28">
         <f t="shared" si="11"/>
-        <v>140.10993129018686</v>
+        <v>-2.1222410836343589E-2</v>
       </c>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
@@ -6871,7 +6871,7 @@
       </c>
       <c r="AN29">
         <f t="shared" si="11"/>
-        <v>140.11018039578528</v>
+        <v>-2.1843599794953573E-2</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
@@ -6980,7 +6980,7 @@
       </c>
       <c r="AN30">
         <f t="shared" si="11"/>
-        <v>140.11043640909583</v>
+        <v>-2.2482014357502706E-2</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
@@ -7089,7 +7089,7 @@
       </c>
       <c r="AN31">
         <f t="shared" si="11"/>
-        <v>140.11069924262335</v>
+        <v>-2.3137436340417029E-2</v>
       </c>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="AN32">
         <f t="shared" si="11"/>
-        <v>140.11096875923482</v>
+        <v>-2.3809523777309612E-2</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="AN33">
         <f t="shared" si="11"/>
-        <v>140.11124476584052</v>
+        <v>-2.4497795165464652E-2</v>
       </c>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
@@ -7416,7 +7416,7 @@
       </c>
       <c r="AN34">
         <f t="shared" si="11"/>
-        <v>140.11152700673983</v>
+        <v>-2.5201612869742006E-2</v>
       </c>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
@@ -7525,7 +7525,7 @@
       </c>
       <c r="AN35">
         <f t="shared" si="11"/>
-        <v>140.11181515669628</v>
+        <v>-2.5920165855331728E-2</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="AN36">
         <f t="shared" si="11"/>
-        <v>140.11210881384133</v>
+        <v>-2.6652451991409667E-2</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -7743,7 +7743,7 @@
       </c>
       <c r="AN37">
         <f t="shared" si="11"/>
-        <v>140.11240749253113</v>
+        <v>-2.7397260239577902E-2</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -7852,7 +7852,7 @@
       </c>
       <c r="AN38">
         <f t="shared" si="11"/>
-        <v>140.11271061631533</v>
+        <v>-2.8153153118580788E-2</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -7961,7 +7961,7 @@
       </c>
       <c r="AN39">
         <f t="shared" si="11"/>
-        <v>140.11301751121272</v>
+        <v>-2.8918449936318816E-2</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
@@ -8070,7 +8070,7 @@
       </c>
       <c r="AN40">
         <f t="shared" si="11"/>
-        <v>140.11332739952562</v>
+        <v>-2.9691211366496013E-2</v>
       </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
@@ -8179,7 +8179,7 @@
       </c>
       <c r="AN41">
         <f t="shared" si="11"/>
-        <v>140.11363939446647</v>
+        <v>-3.0469226046566624E-2</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -8288,7 +8288,7 @@
       </c>
       <c r="AN42">
         <f t="shared" si="11"/>
-        <v>140.113952495901</v>
+        <v>-3.1249999964956532E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>